<commit_message>
Mejoras en los comentarios y renombre algunas variables
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">SKU</t>
   </si>
@@ -50,16 +50,18 @@
   </si>
   <si>
     <t xml:space="preserve">RM 5900/N/S2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3614222915713-0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_ &quot;$ &quot;* #,##0.00_ ;_ &quot;$ &quot;* \-#,##0.00_ ;_ &quot;$ &quot;* \-??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -85,13 +87,13 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -99,7 +101,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -144,13 +146,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -159,15 +161,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="17" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -188,13 +186,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.37"/>
@@ -202,7 +200,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.38"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -216,93 +214,108 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="n">
+      <c r="B2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <f aca="false">B2/1.3</f>
         <v>0.769230769230769</v>
       </c>
-      <c r="D2" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="D2" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="n">
+      <c r="B3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="n">
         <f aca="false">B3/1.3</f>
         <v>0.769230769230769</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="0" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="n">
+      <c r="B4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="n">
         <f aca="false">B4/1.3</f>
         <v>0.769230769230769</v>
       </c>
-      <c r="D4" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="D4" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4" t="n">
+      <c r="B5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="n">
         <f aca="false">B5/1.3</f>
         <v>0.769230769230769</v>
       </c>
-      <c r="D5" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="D5" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="n">
+      <c r="B6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="n">
         <f aca="false">B6/1.3</f>
         <v>0.769230769230769</v>
       </c>
-      <c r="D6" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="D6" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="n">
+      <c r="B7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="n">
         <f aca="false">B7/1.3</f>
         <v>0.769230769230769</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <f aca="false">B8/1.3</f>
+        <v>0.769230769230769</v>
+      </c>
+      <c r="D8" s="0" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modifi excel input file
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -200,10 +200,10 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.37"/>
@@ -230,12 +230,11 @@
         <v>4</v>
       </c>
       <c r="B2" s="5" t="n">
-        <f aca="false">RANDBETWEEN(10,100)</f>
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="C2" s="5" t="n">
         <f aca="false">B2/1.3</f>
-        <v>47.6923076923077</v>
+        <v>76.9230769230769</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>2</v>
@@ -246,12 +245,11 @@
         <v>3351500002122</v>
       </c>
       <c r="B3" s="5" t="n">
-        <f aca="false">RANDBETWEEN(10,100)</f>
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="C3" s="5" t="n">
         <f aca="false">B3/1.3</f>
-        <v>63.0769230769231</v>
+        <v>76.9230769230769</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>10</v>
@@ -262,12 +260,11 @@
         <v>3351500004911</v>
       </c>
       <c r="B4" s="5" t="n">
-        <f aca="false">RANDBETWEEN(10,100)</f>
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C4" s="5" t="n">
         <f aca="false">B4/1.3</f>
-        <v>23.0769230769231</v>
+        <v>76.9230769230769</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>2</v>
@@ -278,12 +275,11 @@
         <v>3351500001590</v>
       </c>
       <c r="B5" s="5" t="n">
-        <f aca="false">RANDBETWEEN(10,100)</f>
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="C5" s="5" t="n">
         <f aca="false">B5/1.3</f>
-        <v>59.2307692307692</v>
+        <v>76.9230769230769</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>2</v>
@@ -294,12 +290,11 @@
         <v>3351500980086</v>
       </c>
       <c r="B6" s="5" t="n">
-        <f aca="false">RANDBETWEEN(10,100)</f>
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C6" s="5" t="n">
         <f aca="false">B6/1.3</f>
-        <v>70</v>
+        <v>76.9230769230769</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>2</v>
@@ -310,12 +305,11 @@
         <v>3351500002703</v>
       </c>
       <c r="B7" s="5" t="n">
-        <f aca="false">RANDBETWEEN(10,100)</f>
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C7" s="5" t="n">
         <f aca="false">B7/1.3</f>
-        <v>67.6923076923077</v>
+        <v>76.9230769230769</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>2</v>
@@ -326,12 +320,11 @@
         <v>3351500002702</v>
       </c>
       <c r="B8" s="5" t="n">
-        <f aca="false">RANDBETWEEN(10,100)</f>
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="C8" s="5" t="n">
         <f aca="false">B8/1.3</f>
-        <v>56.1538461538462</v>
+        <v>76.9230769230769</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>2</v>
@@ -342,12 +335,11 @@
         <v>3351500002696</v>
       </c>
       <c r="B9" s="5" t="n">
-        <f aca="false">RANDBETWEEN(10,100)</f>
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="C9" s="5" t="n">
         <f aca="false">B9/1.3</f>
-        <v>26.9230769230769</v>
+        <v>76.9230769230769</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>2</v>
@@ -358,12 +350,11 @@
         <v>30122604</v>
       </c>
       <c r="B10" s="5" t="n">
-        <f aca="false">RANDBETWEEN(10,100)</f>
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="C10" s="5" t="n">
         <f aca="false">B10/1.3</f>
-        <v>22.3076923076923</v>
+        <v>76.9230769230769</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>2</v>
@@ -374,12 +365,11 @@
         <v>7798125437148</v>
       </c>
       <c r="B11" s="5" t="n">
-        <f aca="false">RANDBETWEEN(10,100)</f>
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="C11" s="5" t="n">
         <f aca="false">B11/1.3</f>
-        <v>20.7692307692308</v>
+        <v>76.9230769230769</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>2</v>
@@ -390,12 +380,11 @@
         <v>8011607294350</v>
       </c>
       <c r="B12" s="5" t="n">
-        <f aca="false">RANDBETWEEN(10,100)</f>
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="C12" s="5" t="n">
         <f aca="false">B12/1.3</f>
-        <v>63.0769230769231</v>
+        <v>76.9230769230769</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>2</v>
@@ -406,12 +395,11 @@
         <v>5</v>
       </c>
       <c r="B13" s="5" t="n">
-        <f aca="false">RANDBETWEEN(10,100)</f>
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="C13" s="5" t="n">
         <f aca="false">B13/1.3</f>
-        <v>11.5384615384615</v>
+        <v>76.9230769230769</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>2</v>
@@ -422,12 +410,11 @@
         <v>6</v>
       </c>
       <c r="B14" s="5" t="n">
-        <f aca="false">RANDBETWEEN(10,100)</f>
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="C14" s="5" t="n">
         <f aca="false">B14/1.3</f>
-        <v>27.6923076923077</v>
+        <v>76.9230769230769</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>2</v>
@@ -438,12 +425,11 @@
         <v>7</v>
       </c>
       <c r="B15" s="5" t="n">
-        <f aca="false">RANDBETWEEN(10,100)</f>
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="C15" s="5" t="n">
         <f aca="false">B15/1.3</f>
-        <v>12.3076923076923</v>
+        <v>76.9230769230769</v>
       </c>
       <c r="D15" s="6" t="n">
         <v>2</v>

</xml_diff>